<commit_message>
added blacksmith and shop to main menu
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03FE19E-C16A-456C-9CB5-A5A9475E1521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A965DE-59C3-4395-916D-A8E8312E7791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>7: marchand</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>les deux</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -152,12 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23022110-3C4A-46F7-A81D-61E9BECFEE4B}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,7 +487,7 @@
     <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -495,23 +495,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -519,7 +525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -527,39 +533,48 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -567,7 +582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -575,7 +590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -583,7 +598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -591,7 +606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -599,7 +614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -607,7 +622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
stats + inventory menu
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A965DE-59C3-4395-916D-A8E8312E7791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA6257-ADA6-4530-8D6F-826C40EDB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>7: marchand</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>esthétique globale</t>
+  </si>
+  <si>
+    <t>Roméo(directeur artistique)</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23022110-3C4A-46F7-A81D-61E9BECFEE4B}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,6 +692,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
structure & init weapon/armor + affichage art
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ebddbe4d49021ac/Bureau/Red-Hunter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA6257-ADA6-4530-8D6F-826C40EDB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DACA6257-ADA6-4530-8D6F-826C40EDB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FD80F49-CB06-468E-AE8F-AC67FE64030D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -483,17 +483,17 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -501,7 +501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -523,7 +523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -531,15 +531,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,7 +550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -558,7 +558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -569,7 +569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -580,7 +580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -588,15 +588,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -604,7 +604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -612,7 +612,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -620,7 +620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -628,7 +628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -636,7 +636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -644,7 +644,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -652,7 +652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -660,7 +660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -668,7 +668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -676,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -684,7 +684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -692,7 +692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
monsters + first items(materials and heals) + skills
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ebddbe4d49021ac/Bureau/Red-Hunter/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DACA6257-ADA6-4530-8D6F-826C40EDB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FD80F49-CB06-468E-AE8F-AC67FE64030D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F615F21-6BAC-4E4F-82EF-6922845A80C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>7: marchand</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Roméo(directeur artistique)</t>
+  </si>
+  <si>
+    <t>merges</t>
+  </si>
+  <si>
+    <t>Fabio(directeur cohésion)</t>
+  </si>
+  <si>
+    <t>Bonus: Qui Sont Ils</t>
   </si>
 </sst>
 </file>
@@ -480,20 +489,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23022110-3C4A-46F7-A81D-61E9BECFEE4B}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="1" max="1" width="32.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -501,7 +510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -523,7 +532,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -531,15 +540,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,7 +562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -558,7 +570,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -569,7 +581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -580,7 +592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -588,23 +600,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -612,15 +630,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -628,7 +649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -636,7 +657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -644,7 +665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -652,7 +673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -660,7 +681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -668,7 +689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -676,7 +697,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -684,7 +705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -692,12 +713,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debut de l'upgrade d'arme
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ebddbe4d49021ac/Bureau/Red-Hunter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DACA6257-ADA6-4530-8D6F-826C40EDB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FD80F49-CB06-468E-AE8F-AC67FE64030D}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{DACA6257-ADA6-4530-8D6F-826C40EDB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE72D1DA-9A07-40B9-A130-90D9C4192472}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>7: marchand</t>
   </si>
@@ -181,6 +181,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23022110-3C4A-46F7-A81D-61E9BECFEE4B}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,6 +607,9 @@
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">

</xml_diff>

<commit_message>
battle (no IA for monsters) + all monsters in game
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F615F21-6BAC-4E4F-82EF-6922845A80C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183C995E-3E2F-4D8C-BD26-7F36EF0A4C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>7: marchand</t>
   </si>
@@ -150,12 +150,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,9 +182,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -491,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23022110-3C4A-46F7-A81D-61E9BECFEE4B}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +529,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -522,7 +540,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -541,7 +559,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -552,7 +570,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -566,12 +584,12 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -582,7 +600,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -601,7 +619,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -612,7 +630,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -631,7 +649,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -642,11 +660,14 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -657,7 +678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -665,7 +686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -673,15 +694,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -689,7 +713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -697,7 +721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -705,7 +729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -713,7 +737,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -721,7 +745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -729,7 +753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Stacking limited for potions + bag ameliorations buyable
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E572CA-C104-4BA0-BD6B-1350630972FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C95F3E-4316-40D0-B834-B7D20A635E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>7: marchand</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Johan</t>
+  </si>
+  <si>
+    <t>perfect</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,6 +191,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,7 +513,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B25"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +554,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -581,11 +587,14 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -648,7 +657,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -749,11 +758,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inventory and shop fixed
</commit_message>
<xml_diff>
--- a/docs/Répartition des taches.xlsx
+++ b/docs/Répartition des taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabib\OneDrive\Bureau\Projet Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F151D2EE-E8D8-4A7D-9FC5-E892B2AB1678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35010627-CF81-4A72-B3E7-6225538184D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{192C6059-E459-4DB7-8886-FF7143910171}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>7: marchand</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Bonus: ASCII Art</t>
-  </si>
-  <si>
-    <t>les deux</t>
   </si>
   <si>
     <t>esthétique globale</t>
@@ -147,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,12 +169,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -191,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,9 +194,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -525,7 +513,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,7 +652,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -704,40 +692,40 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>24</v>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>26</v>
+      <c r="B23" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>23</v>

</xml_diff>